<commit_message>
Add Excel Data Model and update Helpers
</commit_message>
<xml_diff>
--- a/src/main/resources/Template.xlsx
+++ b/src/main/resources/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trelloimigration\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\trello_imigration\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F9965E-93D2-4334-8A3D-124BE496BF6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732A69BF-2C46-4D91-BE34-37386DE424E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>C67981</t>
   </si>
@@ -47,6 +47,21 @@
   </si>
   <si>
     <t>Check bus routing color on Public site - Driver chooses  route 4</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tittle </t>
+  </si>
+  <si>
+    <t>Label</t>
   </si>
 </sst>
 </file>
@@ -887,55 +902,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E5" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>